<commit_message>
Détection des programmes non fonctionnels
</commit_message>
<xml_diff>
--- a/Documents techniques/Liste Applis.xlsx
+++ b/Documents techniques/Liste Applis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Téléchargements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis-clementlangue/Library/Mobile Documents/com~apple~CloudDocs/Cours/CIR3/Projet/Nao/ProjetNao/Documents techniques/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="102_{CF98FAF1-5C4E-433C-B0BE-2DDB4200438C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{A4D269B3-27EE-4D83-957E-5B9066ED75D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D74C22D-A4A8-0E45-84FE-430661EBC306}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{8F314484-7FE2-4D01-AEBB-A661FFCDD328}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" xr2:uid="{8F314484-7FE2-4D01-AEBB-A661FFCDD328}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -867,6 +867,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3566,7 +3569,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3864,33 +3867,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADF1266-C755-4906-ADA5-D303D8AA703C}">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0" xr3:uid="{82E2B05C-9E5C-59B2-87B3-6103991E69CC}">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.85546875" style="4"/>
-    <col min="4" max="4" width="13.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="13.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11.5" style="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="23" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="17" style="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="20" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3907,7 +3910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -3947,21 +3950,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <v>2.8472222222222222E-2</v>
+        <v>0.10555555555555556</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
@@ -4001,21 +4004,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5">
-        <v>0.15</v>
+        <v>2.8472222222222222E-2</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
@@ -4053,21 +4056,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5">
-        <v>0.16180555555555556</v>
+        <v>0.15</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
@@ -4103,21 +4106,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>0.10069444444444443</v>
+        <v>0.10208333333333335</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
@@ -4153,21 +4156,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5">
-        <v>0.13958333333333334</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -4203,21 +4206,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1">
+    <row r="8" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5">
-        <v>0.10486111111111111</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
@@ -4259,21 +4262,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <v>0.10208333333333335</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
@@ -4311,41 +4314,41 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" thickBot="1">
+    <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5">
-        <v>0.10625</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" thickBot="1">
+    <row r="11" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5">
-        <v>0.11458333333333333</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
@@ -4381,21 +4384,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1">
+    <row r="12" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5">
-        <v>0.14305555555555557</v>
+        <v>0.16180555555555556</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -4433,21 +4436,21 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1">
+    <row r="13" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5">
-        <v>0.18194444444444444</v>
+        <v>8.2638888888888887E-2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
@@ -4483,21 +4486,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" thickBot="1">
+    <row r="14" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5">
-        <v>0.10555555555555556</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -4533,21 +4536,21 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1">
+    <row r="15" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="5">
-        <v>0.10208333333333335</v>
+        <v>0.18194444444444444</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>26</v>
+      <c r="E15" s="25" t="s">
+        <v>82</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
@@ -4583,61 +4586,61 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5">
-        <v>0.13472222222222222</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>89</v>
+      <c r="E16" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" thickBot="1">
+    <row r="17" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="5">
-        <v>0.13402777777777777</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1">
+    <row r="18" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="5">
-        <v>0.14097222222222222</v>
+        <v>0.10069444444444443</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
@@ -4671,21 +4674,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1">
+    <row r="19" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="5">
-        <v>0.18194444444444444</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
@@ -4719,21 +4722,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1">
+    <row r="20" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="5">
-        <v>8.2638888888888887E-2</v>
+        <v>0.10486111111111111</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
@@ -4767,21 +4770,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" thickBot="1">
+    <row r="21" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5">
-        <v>0.17847222222222223</v>
+        <v>0.10208333333333335</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>100</v>
+        <v>7</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
@@ -4819,21 +4822,21 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1">
+    <row r="22" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="5">
-        <v>0.13749999999999998</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
@@ -4867,21 +4870,21 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="5">
-        <v>0.1111111111111111</v>
+        <v>0.10625</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
@@ -4915,7 +4918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" thickBot="1">
+    <row r="24" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>97</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" thickBot="1">
+    <row r="25" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -5033,7 +5036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
@@ -5053,7 +5056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
@@ -5073,7 +5076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="15">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>61</v>
       </c>
@@ -5113,7 +5116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
@@ -5126,11 +5129,11 @@
       <c r="D31" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
@@ -5143,14 +5146,14 @@
       <c r="D32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="25" t="s">
         <v>121</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>60</v>
       </c>
@@ -5170,7 +5173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>110</v>
       </c>
@@ -5190,7 +5193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>40</v>
       </c>
@@ -5210,7 +5213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>22</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>113</v>
       </c>
@@ -5247,7 +5250,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>58</v>
       </c>
@@ -5267,7 +5270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>54</v>
       </c>
@@ -5287,7 +5290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
@@ -5307,7 +5310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
@@ -5327,7 +5330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>38</v>
       </c>
@@ -5347,7 +5350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>101</v>
       </c>
@@ -5367,7 +5370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>28</v>
       </c>
@@ -5387,7 +5390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>134</v>
       </c>
@@ -5407,7 +5410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>94</v>
       </c>
@@ -5424,7 +5427,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>104</v>
       </c>
@@ -5441,7 +5444,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>138</v>
       </c>
@@ -5461,7 +5464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>103</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>98</v>
       </c>
@@ -5495,7 +5498,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>17</v>
       </c>
@@ -5515,7 +5518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>143</v>
       </c>
@@ -5532,7 +5535,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>72</v>
       </c>
@@ -5552,41 +5555,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>145</v>
       </c>
       <c r="C54" s="5">
-        <v>1.7361111111111112E-2</v>
+        <v>1.2499999999999999E-2</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E54" s="25"/>
     </row>
-    <row r="55" spans="1:6" ht="15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>145</v>
       </c>
       <c r="C55" s="5">
-        <v>1.2499999999999999E-2</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>149</v>
+        <v>71</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>86</v>
       </c>
@@ -5606,7 +5610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
@@ -5626,7 +5630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>64</v>
       </c>
@@ -5646,7 +5650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>52</v>
       </c>
@@ -5666,7 +5670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>45</v>
       </c>
@@ -5686,7 +5690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>83</v>
       </c>
@@ -5706,7 +5710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
@@ -5723,7 +5727,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>27</v>
       </c>
@@ -5736,14 +5740,14 @@
       <c r="D63" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="25" t="s">
         <v>158</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>159</v>
       </c>
@@ -5763,39 +5767,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:9">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="2:9">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" s="6"/>
       <c r="G73" s="20"/>
     </row>
-    <row r="74" spans="2:9">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" s="6"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="2:9">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="2:9">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="2:9">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="2:9">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="2:9">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F61" xr:uid="{F721E9AF-9819-471B-A393-691D375F3842}">
-    <sortState ref="A2:F64">
-      <sortCondition ref="B1:B61"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
+      <sortCondition ref="B1:B64"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A1:P60">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:P60">
     <sortCondition ref="C44"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>